<commit_message>
Updated FP & effort table.
</commit_message>
<xml_diff>
--- a/documentation/UseCaseTimeEstimation.xlsx
+++ b/documentation/UseCaseTimeEstimation.xlsx
@@ -79,7 +79,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[h]:mm"/>
+    <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -147,7 +147,7 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -196,7 +196,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="165" formatCode="[h]:mm"/>
+      <numFmt numFmtId="164" formatCode="[h]:mm"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -327,7 +327,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="165" formatCode="[h]:mm"/>
+      <numFmt numFmtId="164" formatCode="[h]:mm"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -671,16 +671,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>11.7</c:v>
+                  <c:v>16.38</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.7</c:v>
+                  <c:v>16.38</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.4</c:v>
+                  <c:v>32.76</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.1</c:v>
+                  <c:v>16.38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -727,10 +727,10 @@
                 <c:formatCode>h:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.2638888888888889</c:v>
+                  <c:v>0.24305555555555555</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.21527777777777779</c:v>
+                  <c:v>0.1875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -742,7 +742,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>22.1</c:v>
+                  <c:v>26.39</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>13.65</c:v>
@@ -815,6 +815,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-9894-4A3E-9592-5B4398B5A735}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:xVal>
             <c:numRef>
@@ -835,7 +840,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5.85</c:v>
+                  <c:v>8.19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2086,7 +2091,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2140,7 +2145,7 @@
         <v>0.22222222222222224</v>
       </c>
       <c r="G2" s="5">
-        <v>5.85</v>
+        <v>8.19</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2164,7 +2169,7 @@
         <v>0.20833333333333331</v>
       </c>
       <c r="G3" s="5">
-        <v>11.7</v>
+        <v>16.38</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2188,7 +2193,7 @@
         <v>0.1875</v>
       </c>
       <c r="G4" s="5">
-        <v>11.7</v>
+        <v>16.38</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2212,7 +2217,7 @@
         <v>0.25694444444444442</v>
       </c>
       <c r="G5" s="5">
-        <v>23.4</v>
+        <v>32.76</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2236,7 +2241,7 @@
         <v>0.22222222222222221</v>
       </c>
       <c r="G6" s="5">
-        <v>9.1</v>
+        <v>16.38</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2263,7 +2268,7 @@
       </c>
       <c r="G7" s="7">
         <f>SUM(Tabelle1[FP])</f>
-        <v>61.749999999999993</v>
+        <v>90.09</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2298,10 +2303,10 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="4">
-        <v>0.2638888888888889</v>
+        <v>0.24305555555555555</v>
       </c>
       <c r="G10" s="5">
-        <v>22.1</v>
+        <v>26.39</v>
       </c>
       <c r="H10" s="10" t="s">
         <v>15</v>
@@ -2316,7 +2321,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="4">
-        <v>0.21527777777777779</v>
+        <v>0.1875</v>
       </c>
       <c r="G11" s="5">
         <v>13.65</v>
@@ -2345,11 +2350,11 @@
       </c>
       <c r="F12" s="8">
         <f>SUM(Tabelle13[Total])</f>
-        <v>0.47916666666666669</v>
+        <v>0.43055555555555558</v>
       </c>
       <c r="G12" s="7">
         <f>SUM(Tabelle13[FP])</f>
-        <v>35.75</v>
+        <v>40.04</v>
       </c>
       <c r="H12" s="9"/>
     </row>

</xml_diff>

<commit_message>
added det, ret calculaction.
</commit_message>
<xml_diff>
--- a/documentation/UseCaseTimeEstimation.xlsx
+++ b/documentation/UseCaseTimeEstimation.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12780" windowHeight="5445"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12780" windowHeight="5445" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="32">
   <si>
     <t>Documentation</t>
   </si>
@@ -72,6 +73,54 @@
   </si>
   <si>
     <t>Time is estimated.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RET </t>
+  </si>
+  <si>
+    <t>recorded element type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DET </t>
+  </si>
+  <si>
+    <t>data element type</t>
+  </si>
+  <si>
+    <t>user recognizable subgroup of data</t>
+  </si>
+  <si>
+    <t>unique user recognizable, non-repeated field maintained or retrieved</t>
+  </si>
+  <si>
+    <t>FTR</t>
+  </si>
+  <si>
+    <t>Measurement Parameter</t>
+  </si>
+  <si>
+    <t>RET</t>
+  </si>
+  <si>
+    <t>Number of user input</t>
+  </si>
+  <si>
+    <t>Number of user output</t>
+  </si>
+  <si>
+    <t>Number of user inquiries</t>
+  </si>
+  <si>
+    <t>Number of files</t>
+  </si>
+  <si>
+    <t>Number of external interfaces</t>
+  </si>
+  <si>
+    <t>file type referenced</t>
+  </si>
+  <si>
+    <t>Moveright</t>
   </si>
 </sst>
 </file>
@@ -181,6 +230,9 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -202,16 +254,13 @@
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FFFF0000"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
@@ -238,6 +287,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -250,6 +303,135 @@
         <vertAlign val="baseline"/>
         <sz val="11"/>
         <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="[h]:mm"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
@@ -276,76 +458,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="[h]:mm"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="25" formatCode="hh:mm"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -369,21 +481,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="25" formatCode="hh:mm"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -407,6 +504,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -422,35 +523,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="25" formatCode="hh:mm"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -461,42 +533,19 @@
     <dxf>
       <font>
         <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1767,28 +1816,76 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266701</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>706153</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>153651</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1028701" y="866775"/>
+          <a:ext cx="4935252" cy="7478376"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:G7" totalsRowCount="1" totalsRowDxfId="27">
   <autoFilter ref="A1:G6"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Old Use Cases" totalsRowDxfId="13"/>
-    <tableColumn id="2" name="Documentation" totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="12">
+    <tableColumn id="1" name="Old Use Cases" totalsRowDxfId="26"/>
+    <tableColumn id="2" name="Documentation" totalsRowFunction="custom" dataDxfId="25" totalsRowDxfId="24">
       <totalsRowFormula>SUM(Tabelle1[Documentation])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" name="Coding" totalsRowFunction="custom" dataDxfId="25" totalsRowDxfId="11">
+    <tableColumn id="3" name="Coding" totalsRowFunction="custom" dataDxfId="23" totalsRowDxfId="22">
       <totalsRowFormula>SUM(Tabelle1[Coding])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" name="Testing" totalsRowFunction="custom" dataDxfId="24" totalsRowDxfId="10">
+    <tableColumn id="4" name="Testing" totalsRowFunction="custom" dataDxfId="21" totalsRowDxfId="20">
       <totalsRowFormula>SUM(Tabelle1[Testing])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="Warm-Up time " totalsRowFunction="custom" dataDxfId="23" totalsRowDxfId="9">
+    <tableColumn id="5" name="Warm-Up time " totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="18">
       <totalsRowFormula>SUM(Tabelle1[Warm-Up time ])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="Total" totalsRowFunction="custom" dataDxfId="22" totalsRowDxfId="8">
+    <tableColumn id="6" name="Total" totalsRowFunction="custom" dataDxfId="17" totalsRowDxfId="16">
       <calculatedColumnFormula>SUM(B2:E2)</calculatedColumnFormula>
       <totalsRowFormula>SUM(Tabelle1[Total])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" name="FP" totalsRowFunction="custom" dataDxfId="21" totalsRowDxfId="7">
+    <tableColumn id="7" name="FP" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="14">
       <totalsRowFormula>SUM(Tabelle1[FP])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -1797,27 +1894,27 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle13" displayName="Tabelle13" ref="A9:G12" totalsRowCount="1" totalsRowDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle13" displayName="Tabelle13" ref="A9:G12" totalsRowCount="1" totalsRowDxfId="13">
   <autoFilter ref="A9:G11"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="New Use Cases" totalsRowDxfId="6"/>
-    <tableColumn id="2" name="Documentation" totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="5">
+    <tableColumn id="1" name="New Use Cases" totalsRowDxfId="12"/>
+    <tableColumn id="2" name="Documentation" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
       <totalsRowFormula>SUM(Tabelle13[Documentation])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" name="Coding" totalsRowFunction="custom" dataDxfId="18" totalsRowDxfId="4">
+    <tableColumn id="3" name="Coding" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="8">
       <totalsRowFormula>SUM(Tabelle13[Coding])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" name="Testing" totalsRowFunction="custom" dataDxfId="17" totalsRowDxfId="3">
+    <tableColumn id="4" name="Testing" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="6">
       <totalsRowFormula>SUM(Tabelle13[Testing])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="Warm-Up time " totalsRowFunction="custom" dataDxfId="16" totalsRowDxfId="2">
+    <tableColumn id="5" name="Warm-Up time " totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="4">
       <totalsRowFormula>SUM(Tabelle13[Warm-Up time ])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="Total" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="1">
+    <tableColumn id="6" name="Total" totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="2">
       <calculatedColumnFormula>SUM(B10:E10)</calculatedColumnFormula>
       <totalsRowFormula>SUM(Tabelle13[Total])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" name="FP" totalsRowFunction="custom" dataDxfId="14" totalsRowDxfId="0">
+    <tableColumn id="7" name="FP" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="0">
       <totalsRowFormula>SUM(Tabelle13[FP])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -2090,7 +2187,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
@@ -2367,4 +2464,489 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:O40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L12" t="s">
+        <v>29</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="K14" t="s">
+        <v>7</v>
+      </c>
+      <c r="L14" t="s">
+        <v>23</v>
+      </c>
+      <c r="M14" t="s">
+        <v>18</v>
+      </c>
+      <c r="N14" t="s">
+        <v>24</v>
+      </c>
+      <c r="O14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M15">
+        <v>2</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L16" t="s">
+        <v>26</v>
+      </c>
+      <c r="M16">
+        <v>2</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L17" t="s">
+        <v>27</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L18" t="s">
+        <v>28</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L19" t="s">
+        <v>29</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K21" t="s">
+        <v>31</v>
+      </c>
+      <c r="L21" t="s">
+        <v>23</v>
+      </c>
+      <c r="M21" t="s">
+        <v>18</v>
+      </c>
+      <c r="N21" t="s">
+        <v>24</v>
+      </c>
+      <c r="O21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L22" t="s">
+        <v>25</v>
+      </c>
+      <c r="M22">
+        <v>2</v>
+      </c>
+      <c r="N22">
+        <v>2</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L23" t="s">
+        <v>26</v>
+      </c>
+      <c r="M23">
+        <v>2</v>
+      </c>
+      <c r="N23">
+        <v>2</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L24" t="s">
+        <v>27</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L25" t="s">
+        <v>28</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L26" t="s">
+        <v>29</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K28" t="s">
+        <v>9</v>
+      </c>
+      <c r="L28" t="s">
+        <v>23</v>
+      </c>
+      <c r="M28" t="s">
+        <v>18</v>
+      </c>
+      <c r="N28" t="s">
+        <v>24</v>
+      </c>
+      <c r="O28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L29" t="s">
+        <v>25</v>
+      </c>
+      <c r="M29">
+        <v>4</v>
+      </c>
+      <c r="N29">
+        <v>1</v>
+      </c>
+      <c r="O29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L30" t="s">
+        <v>26</v>
+      </c>
+      <c r="M30">
+        <v>4</v>
+      </c>
+      <c r="N30">
+        <v>1</v>
+      </c>
+      <c r="O30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L31" t="s">
+        <v>27</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L32" t="s">
+        <v>28</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L33" t="s">
+        <v>29</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K35" t="s">
+        <v>10</v>
+      </c>
+      <c r="L35" t="s">
+        <v>23</v>
+      </c>
+      <c r="M35" t="s">
+        <v>18</v>
+      </c>
+      <c r="N35" t="s">
+        <v>24</v>
+      </c>
+      <c r="O35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L36" t="s">
+        <v>25</v>
+      </c>
+      <c r="M36">
+        <v>2</v>
+      </c>
+      <c r="N36">
+        <v>1</v>
+      </c>
+      <c r="O36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L37" t="s">
+        <v>26</v>
+      </c>
+      <c r="M37">
+        <v>2</v>
+      </c>
+      <c r="N37">
+        <v>1</v>
+      </c>
+      <c r="O37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L38" t="s">
+        <v>27</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L39" t="s">
+        <v>28</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L40" t="s">
+        <v>29</v>
+      </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>